<commit_message>
chore: evaluate weekly results
</commit_message>
<xml_diff>
--- a/DoubleBottomOverview.xlsx
+++ b/DoubleBottomOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thorstenmueller/stockAlgo/DB-RSI-Divergence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B797413-C96A-DB43-966F-CA683B00AE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F0B929-D72E-5D41-9DAE-EEF2965B253E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40520" yWindow="1780" windowWidth="34820" windowHeight="21500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-56820" yWindow="8840" windowWidth="34820" windowHeight="21500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="97">
   <si>
     <t>Ticker</t>
   </si>
@@ -322,13 +322,16 @@
   </si>
   <si>
     <t>Ergebnisse Algo</t>
+  </si>
+  <si>
+    <t>=WENN(UND([@[Trend vorher vorhanden]]="ja";WENN(ODER([@[RSI Divergenz]]="ja";[@[DB / DT]]="ja");WAHR; FALSCH));WAHR; FALSCH)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +355,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -417,10 +427,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -435,18 +446,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -455,6 +483,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -474,18 +514,6 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -500,13 +528,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4162D173-E466-6F42-A4EA-0B5FBDAE63A2}" name="Tabelle2" displayName="Tabelle2" ref="A2:J18" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4162D173-E466-6F42-A4EA-0B5FBDAE63A2}" name="Tabelle2" displayName="Tabelle2" ref="A2:J18" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A2:J18" xr:uid="{4162D173-E466-6F42-A4EA-0B5FBDAE63A2}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{86E29E93-B080-4D40-88A6-CA0AD9DDCCEA}" name="Woche"/>
     <tableColumn id="2" xr3:uid="{4918E6F0-7D7E-4247-BD38-9AAB7BB688FE}" name="Ergebnisse"/>
-    <tableColumn id="3" xr3:uid="{B3DC2B1F-27FD-AF45-A3FF-79420A6B9DA7}" name="Ergebnisse bestätigt" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{AFA19266-B13A-0547-9792-9E2929257B30}" name="Spalte1" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{B3DC2B1F-27FD-AF45-A3FF-79420A6B9DA7}" name="Ergebnisse bestätigt" dataDxfId="12"/>
+    <tableColumn id="19" xr3:uid="{AFA19266-B13A-0547-9792-9E2929257B30}" name="Spalte1" dataDxfId="11">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{1AA4EDA5-B0AF-F44C-9FB3-E9826C38477A}" name="Anz Trades / gehandelt"/>
@@ -521,18 +549,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6235039E-C30D-434F-949D-3A0FC1457667}" name="Tabelle24" displayName="Tabelle24" ref="L2:U18" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6235039E-C30D-434F-949D-3A0FC1457667}" name="Tabelle24" displayName="Tabelle24" ref="L2:U18" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="L2:U18" xr:uid="{6235039E-C30D-434F-949D-3A0FC1457667}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{2FBB2397-D236-D841-A1B0-A172F73867DA}" name="Woche"/>
     <tableColumn id="2" xr3:uid="{FDA151B0-26EA-D042-AEDF-F2D62BBEA64F}" name="Ergebnisse"/>
-    <tableColumn id="3" xr3:uid="{5762EFCC-38EC-8A48-8E4D-172DC9B06A1D}" name="Ergebnisse bestätigt" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{959C4F92-7318-1B4B-A4C5-EE3D8BA7C4D8}" name="Spalte1" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{5762EFCC-38EC-8A48-8E4D-172DC9B06A1D}" name="Ergebnisse bestätigt" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{959C4F92-7318-1B4B-A4C5-EE3D8BA7C4D8}" name="Spalte1" dataDxfId="8">
       <calculatedColumnFormula>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{16130ADC-F53C-3B4F-BD85-8138E18EC422}" name="Anz Trades / gehandelt"/>
     <tableColumn id="5" xr3:uid="{DC193C7E-6C97-2D4B-B4E8-A8538861E67D}" name="Anz Gewinntrades"/>
-    <tableColumn id="7" xr3:uid="{88A47F7E-7680-E54C-8F17-13CF36C8F6BF}" name="Gewinn"/>
+    <tableColumn id="7" xr3:uid="{88A47F7E-7680-E54C-8F17-13CF36C8F6BF}" name="Gewinn" dataDxfId="6">
+      <calculatedColumnFormula>SUBTOTAL(101,Tabelle1[GuV (closing zum closing)])</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="8" xr3:uid="{8BA1E6FB-F6E3-744B-9D02-286F52110E11}" name="Anz Verlusttrades"/>
     <tableColumn id="9" xr3:uid="{9A514872-A1AF-A44F-9792-E49EDFAD66B1}" name="Haltedauer2"/>
     <tableColumn id="10" xr3:uid="{B469D793-282A-CF4D-863F-9A5A8529CF04}" name="Verlust"/>
@@ -542,7 +572,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{703DFFA0-C5A7-B54E-9BD2-0CE249391F34}" name="Tabelle1" displayName="Tabelle1" ref="A1:T46" totalsRowCount="1" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{703DFFA0-C5A7-B54E-9BD2-0CE249391F34}" name="Tabelle1" displayName="Tabelle1" ref="A1:T46" totalsRowCount="1" headerRowDxfId="7">
   <autoFilter ref="A1:T45" xr:uid="{703DFFA0-C5A7-B54E-9BD2-0CE249391F34}">
     <filterColumn colId="10">
       <filters>
@@ -555,13 +585,13 @@
     <tableColumn id="21" xr3:uid="{79261762-C34F-8749-A493-B32FCFA340B0}" name="Market"/>
     <tableColumn id="2" xr3:uid="{CDE762A1-7BE3-4A40-BB2A-F1D859C9AB2C}" name="Date1"/>
     <tableColumn id="3" xr3:uid="{120F138A-24D2-F94B-9F00-522C64990733}" name="Date2"/>
-    <tableColumn id="4" xr3:uid="{E8C8A1B3-C6FD-0F40-B921-15BC21329E77}" name="Course Differenz in %" totalsRowFunction="average" dataDxfId="12" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{CB216F63-570B-E444-B993-98FA238DFAE9}" name="RSI Differenz in %" totalsRowFunction="average" dataDxfId="11" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E8C8A1B3-C6FD-0F40-B921-15BC21329E77}" name="Course Differenz in %" totalsRowFunction="average" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{CB216F63-570B-E444-B993-98FA238DFAE9}" name="RSI Differenz in %" totalsRowFunction="average" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="6" xr3:uid="{FA55C16E-42C0-5A4C-AB1F-901AFA0E1DAA}" name="DB / DT"/>
     <tableColumn id="7" xr3:uid="{F90DC60E-3B8C-EF4B-B73B-60CB789FFD54}" name="RSI Divergenz"/>
     <tableColumn id="14" xr3:uid="{ED9E96C6-D2C4-4D48-BDF0-EFBF572D7820}" name="Grund falls nicht"/>
     <tableColumn id="8" xr3:uid="{60ABAA29-B79B-E34E-A9E7-409E0CEDA8BD}" name="Trend vorher vorhanden"/>
-    <tableColumn id="20" xr3:uid="{81662B82-46D9-1C42-90A1-34C383E69A40}" name="Gehandelt" dataDxfId="9" totalsRowDxfId="0">
+    <tableColumn id="20" xr3:uid="{81662B82-46D9-1C42-90A1-34C383E69A40}" name="Gehandelt" dataDxfId="1">
       <calculatedColumnFormula>IF(AND(Tabelle1[[#This Row],[Trend vorher vorhanden]]="ja",IF(OR(Tabelle1[[#This Row],[RSI Divergenz]]="ja",Tabelle1[[#This Row],[DB / DT]]="ja"),TRUE, FALSE)),TRUE, FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{1BCA9077-C7F4-4F4E-9E2B-447C0AEE3047}" name="Treffer"/>
@@ -569,7 +599,7 @@
     <tableColumn id="11" xr3:uid="{0B6AFD1C-2AD0-A049-9A5C-0B97816823DB}" name="Nach wie vielen Tagen ist es gestiegen" totalsRowFunction="average"/>
     <tableColumn id="12" xr3:uid="{E45F25F8-CEE8-0549-A56F-80268D60DC81}" name="Wieviel % ist der Kurs gedippt bevor er stieg (closing)" totalsRowFunction="average"/>
     <tableColumn id="17" xr3:uid="{65986347-9CD6-A940-A5E0-5E165124E1E9}" name="Wieviel % ist der Kurs gedippt bevor er stieg (low)" totalsRowFunction="average"/>
-    <tableColumn id="15" xr3:uid="{8181BA18-B9A4-494F-9F2F-138029B7E35B}" name="GuV (closing zum closing)" totalsRowFunction="average"/>
+    <tableColumn id="15" xr3:uid="{8181BA18-B9A4-494F-9F2F-138029B7E35B}" name="GuV (closing zum closing)" totalsRowFunction="average" totalsRowDxfId="0" totalsRowCellStyle="Prozent"/>
     <tableColumn id="13" xr3:uid="{FC937719-8A1D-3F42-A808-D38513603A0D}" name="Stieg es danach weiter"/>
     <tableColumn id="18" xr3:uid="{3F170D5E-DB7D-F44C-91B0-6A8D4082039E}" name="Anstieg danach bis zur ersten roten Kerze (closing)"/>
     <tableColumn id="16" xr3:uid="{D1F0796D-3B8C-C444-A9CF-4E705094C73F}" name="Spalte1"/>
@@ -899,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABF0604-F081-2A41-A64F-9BE7E1FBBA34}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -970,6 +1000,11 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -979,15 +1014,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF75EAC-33D2-5749-97C4-A3043BE15CDB}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="8" max="8" width="16.5" customWidth="1"/>
@@ -995,30 +1029,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="L1" s="8" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="L1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" spans="1:21" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1027,7 +1061,7 @@
       <c r="B2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1057,7 +1091,7 @@
       <c r="M2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="2" t="s">
         <v>87</v>
       </c>
       <c r="O2" s="2" t="s">
@@ -1089,7 +1123,7 @@
       <c r="B3">
         <v>19</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3">
         <v>43</v>
       </c>
       <c r="D3" s="1">
@@ -1105,12 +1139,25 @@
       <c r="M3">
         <v>19</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3">
         <v>43</v>
       </c>
       <c r="O3" s="1">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>0.44186046511627908</v>
+      </c>
+      <c r="P3">
+        <v>19</v>
+      </c>
+      <c r="Q3">
+        <v>19</v>
+      </c>
+      <c r="R3" s="7">
+        <f>SUBTOTAL(101,Tabelle1[GuV (closing zum closing)])</f>
+        <v>6.855555555555555E-2</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -1118,165 +1165,165 @@
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N4" s="7"/>
       <c r="O4" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D5" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N5" s="7"/>
       <c r="O5" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D6" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="7"/>
       <c r="O6" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D7" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N7" s="7"/>
       <c r="O7" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D8" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N8" s="7"/>
       <c r="O8" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D9" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N9" s="7"/>
       <c r="O9" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D10" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N10" s="7"/>
       <c r="O10" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D11" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N11" s="7"/>
       <c r="O11" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D12" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N12" s="7"/>
       <c r="O12" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D13" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N13" s="7"/>
       <c r="O13" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D14" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N14" s="7"/>
       <c r="O14" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D15" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N15" s="7"/>
       <c r="O15" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D16" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N16" s="7"/>
       <c r="O16" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D17" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N17" s="7"/>
       <c r="O17" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D18" t="e">
         <f>Tabelle2[[#This Row],[Ergebnisse]]/Tabelle2[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="7"/>
       <c r="O18" t="e">
         <f>Tabelle24[[#This Row],[Ergebnisse]]/Tabelle24[[#This Row],[Ergebnisse bestätigt]]</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="R18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1293,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:T48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1423,8 +1470,8 @@
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="Q2">
-        <v>0.8</v>
+      <c r="Q2" s="1">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="R2" t="s">
         <v>60</v>
@@ -1516,8 +1563,8 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="Q4">
-        <v>4.2</v>
+      <c r="Q4" s="1">
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
@@ -1648,8 +1695,8 @@
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="Q7">
-        <v>0.7</v>
+      <c r="Q7" s="1">
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -1699,8 +1746,8 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="Q8">
-        <v>0.7</v>
+      <c r="Q8" s="1">
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
@@ -1780,8 +1827,8 @@
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="Q10">
-        <v>5.3</v>
+      <c r="Q10" s="1">
+        <v>5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
@@ -1996,8 +2043,8 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="Q16">
-        <v>6.7</v>
+      <c r="Q16" s="1">
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -2047,8 +2094,8 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="Q17">
-        <v>8</v>
+      <c r="Q17" s="1">
+        <v>0.08</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -2098,8 +2145,8 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="Q18">
-        <v>8</v>
+      <c r="Q18" s="1">
+        <v>0.08</v>
       </c>
       <c r="T18" t="s">
         <v>72</v>
@@ -2152,8 +2199,8 @@
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="Q19">
-        <v>7.5</v>
+      <c r="Q19" s="1">
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="T19" t="s">
         <v>73</v>
@@ -2206,8 +2253,8 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="Q20">
-        <v>7.5</v>
+      <c r="Q20" s="1">
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="T20" t="s">
         <v>74</v>
@@ -2260,8 +2307,8 @@
       <c r="P21">
         <v>4.5</v>
       </c>
-      <c r="Q21">
-        <v>15.5</v>
+      <c r="Q21" s="1">
+        <v>0.155</v>
       </c>
       <c r="T21" t="s">
         <v>77</v>
@@ -2377,8 +2424,8 @@
       <c r="P24">
         <v>0</v>
       </c>
-      <c r="Q24">
-        <v>3</v>
+      <c r="Q24" s="1">
+        <v>0.03</v>
       </c>
       <c r="R24" t="s">
         <v>60</v>
@@ -2527,8 +2574,8 @@
       <c r="P28">
         <v>2</v>
       </c>
-      <c r="Q28">
-        <v>1.2</v>
+      <c r="Q28" s="1">
+        <v>1.2E-2</v>
       </c>
       <c r="R28" t="s">
         <v>60</v>
@@ -2737,9 +2784,7 @@
       <c r="P34">
         <v>0</v>
       </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
+      <c r="Q34" s="1"/>
       <c r="R34" t="s">
         <v>60</v>
       </c>
@@ -2800,8 +2845,8 @@
       <c r="P35">
         <v>0</v>
       </c>
-      <c r="Q35">
-        <v>7.2</v>
+      <c r="Q35" s="1">
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="T35" t="s">
         <v>77</v>
@@ -2887,8 +2932,8 @@
       <c r="P37">
         <v>0</v>
       </c>
-      <c r="Q37">
-        <v>11</v>
+      <c r="Q37" s="1">
+        <v>0.11</v>
       </c>
       <c r="T37" t="s">
         <v>77</v>
@@ -2995,8 +3040,8 @@
       <c r="P40">
         <v>0</v>
       </c>
-      <c r="Q40">
-        <v>5.3</v>
+      <c r="Q40" s="1">
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="T40" t="s">
         <v>77</v>
@@ -3049,8 +3094,8 @@
       <c r="P41">
         <v>0</v>
       </c>
-      <c r="Q41">
-        <v>6.9</v>
+      <c r="Q41" s="1">
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
@@ -3163,8 +3208,8 @@
       <c r="P44">
         <v>0</v>
       </c>
-      <c r="Q44">
-        <v>23.9</v>
+      <c r="Q44" s="1">
+        <v>0.23899999999999999</v>
       </c>
       <c r="T44" t="s">
         <v>77</v>
@@ -3209,7 +3254,6 @@
         <f>SUBTOTAL(101,Tabelle1[RSI Differenz in %])</f>
         <v>0.15761373363580503</v>
       </c>
-      <c r="K46" s="7"/>
       <c r="M46">
         <f>SUBTOTAL(101,Tabelle1[Tage bis zur ersten roten Kerze])</f>
         <v>1.1111111111111112</v>
@@ -3226,10 +3270,13 @@
         <f>SUBTOTAL(101,Tabelle1[Wieviel % ist der Kurs gedippt bevor er stieg (low)])</f>
         <v>0.72222222222222221</v>
       </c>
-      <c r="Q46">
+      <c r="Q46" s="7">
         <f>SUBTOTAL(101,Tabelle1[GuV (closing zum closing)])</f>
-        <v>6.4947368421052634</v>
-      </c>
+        <v>6.855555555555555E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q48" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>